<commit_message>
increase pipe finite elements to 4
</commit_message>
<xml_diff>
--- a/gas_net/data/data_files/Gaslib_40/networkData.xlsx
+++ b/gas_net/data/data_files/Gaslib_40/networkData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssnaik\Biegler\gas_networks_italy\gas_networks\gas_net\data\data_files\Gaslib_40\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF455EA-4B59-4432-8CD4-CA45D22971D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B148A5-1554-4CDF-8470-8729C0B6EFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -708,13 +708,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -755,7 +755,7 @@
         <v>7.1514568006000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -775,7 +775,7 @@
         <v>6.40592572072</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -795,7 +795,7 @@
         <v>8.4621655320400002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -815,7 +815,7 @@
         <v>6.9854010493200001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -835,7 +835,7 @@
         <v>7.4443755311900004</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -855,7 +855,7 @@
         <v>6.73248116159</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -875,7 +875,7 @@
         <v>8.9411702828399999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -895,7 +895,7 @@
         <v>8.5833395540000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -915,7 +915,7 @@
         <v>7.3753776974200003</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -935,7 +935,7 @@
         <v>7.1753586073599998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -955,7 +955,7 @@
         <v>6.7041298791399999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -975,7 +975,7 @@
         <v>7.3914117238100001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -995,7 +995,7 @@
         <v>8.42123710095</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>7.0605075488400004</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>7.4457078406599999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>6.68272868748</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>8.90117691783</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>6.9707746782799997</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>6.8901153727300004</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>7.1600196325600001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>8.5229746891700007</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>9.4346584907499995</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>7.53102691462</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>6.0379656315299997</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>8.9727930560200004</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>6.8375660756499999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>7.2972825175800002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>6.0766343127700004</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>7.0121622871099998</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>6.9910068056399997</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>7.3343218248599999</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>7.1259504410399996</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>7.2293030868199999</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>8.2267773593700007</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>8.5682177229499992</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>6.6172322377899997</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>6.5567145582800004</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>6.6466959069599998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>6.4827114548100004</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1553,13 +1553,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>46</v>
@@ -1592,7 +1592,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>18.567399999999999</v>
@@ -1627,7 +1627,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>18.567399999999999</v>
@@ -1662,7 +1662,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>18.567399999999999</v>
@@ -1697,7 +1697,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>18.567399999999999</v>
@@ -1732,7 +1732,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>18.567399999999999</v>
@@ -1767,7 +1767,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <v>18.567399999999999</v>
@@ -1802,7 +1802,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <v>18.567399999999999</v>
@@ -1837,7 +1837,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9">
         <v>18.567399999999999</v>
@@ -1872,7 +1872,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <v>18.567399999999999</v>
@@ -1907,7 +1907,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>18.567399999999999</v>
@@ -1942,7 +1942,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>18.567399999999999</v>
@@ -1977,7 +1977,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <v>18.567399999999999</v>
@@ -2012,7 +2012,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>18.567399999999999</v>
@@ -2047,7 +2047,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <v>18.567399999999999</v>
@@ -2082,7 +2082,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <v>18.567399999999999</v>
@@ -2117,7 +2117,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <v>18.567399999999999</v>
@@ -2152,7 +2152,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>18.567399999999999</v>
@@ -2187,7 +2187,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <v>18.567399999999999</v>
@@ -2222,7 +2222,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <v>18.567399999999999</v>
@@ -2257,7 +2257,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>18.567399999999999</v>
@@ -2292,7 +2292,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>18.567399999999999</v>
@@ -2327,7 +2327,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <v>18.567399999999999</v>
@@ -2362,7 +2362,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <v>18.567399999999999</v>
@@ -2397,7 +2397,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <v>18.567399999999999</v>
@@ -2432,7 +2432,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>18.567399999999999</v>
@@ -2467,7 +2467,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <v>18.567399999999999</v>
@@ -2502,7 +2502,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <v>18.567399999999999</v>
@@ -2537,7 +2537,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <v>18.567399999999999</v>
@@ -2572,7 +2572,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>18.567399999999999</v>
@@ -2607,7 +2607,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <v>18.567399999999999</v>
@@ -2642,7 +2642,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <v>18.567399999999999</v>
@@ -2677,7 +2677,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H33">
         <v>18.567399999999999</v>
@@ -2712,7 +2712,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <v>18.567399999999999</v>
@@ -2747,7 +2747,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H35">
         <v>18.567399999999999</v>
@@ -2782,7 +2782,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H36">
         <v>18.567399999999999</v>
@@ -2817,7 +2817,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37">
         <v>18.567399999999999</v>
@@ -2852,7 +2852,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H38">
         <v>18.567399999999999</v>
@@ -2887,7 +2887,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H39">
         <v>18.567399999999999</v>
@@ -2922,7 +2922,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H40">
         <v>18.567399999999999</v>
@@ -2968,9 +2968,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>95</v>
@@ -2985,7 +2985,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>2424387224.3367658</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>2424387224.3367658</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>2424387224.3367658</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>2424387224.3367658</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>2424387224.3367658</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -3080,9 +3080,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -3091,7 +3091,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>104</v>
       </c>

</xml_diff>